<commit_message>
improve the analysis of heads
</commit_message>
<xml_diff>
--- a/data/regions.xlsx
+++ b/data/regions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\komickn\Documents\src\CTC_Analysis\chinook_sport_central\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5DE1832-0CBD-455D-8C5F-4DEBE7EEB497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{574D2E9B-DA83-4AA9-81C2-AEF4476D2926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0E6B1A2C-CD49-44AB-BFC0-F567D14E751E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0E6B1A2C-CD49-44AB-BFC0-F567D14E751E}"/>
   </bookViews>
   <sheets>
     <sheet name="Area" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="196">
   <si>
     <t>AREA</t>
   </si>
@@ -618,6 +618,15 @@
   </si>
   <si>
     <t>NWCVI S SUMMER ISBM</t>
+  </si>
+  <si>
+    <t>NBC ISBM S FALL</t>
+  </si>
+  <si>
+    <t>NBC ISBM S SPRING</t>
+  </si>
+  <si>
+    <t>NBC ISBM S SUMMER</t>
   </si>
 </sst>
 </file>
@@ -972,7 +981,7 @@
   <dimension ref="A1:E256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C256" sqref="C256:D256"/>
+      <selection activeCell="F95" sqref="F95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2154,7 +2163,7 @@
         <v>12</v>
       </c>
       <c r="E69" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -2171,7 +2180,7 @@
         <v>12</v>
       </c>
       <c r="E70" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -2256,7 +2265,7 @@
         <v>12</v>
       </c>
       <c r="E75" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -2273,7 +2282,7 @@
         <v>12</v>
       </c>
       <c r="E76" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2290,7 +2299,7 @@
         <v>12</v>
       </c>
       <c r="E77" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -2341,7 +2350,7 @@
         <v>12</v>
       </c>
       <c r="E80" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -2358,7 +2367,7 @@
         <v>12</v>
       </c>
       <c r="E81" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -2375,7 +2384,7 @@
         <v>12</v>
       </c>
       <c r="E82" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -2460,7 +2469,7 @@
         <v>4</v>
       </c>
       <c r="E87" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -2477,7 +2486,7 @@
         <v>4</v>
       </c>
       <c r="E88" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -2562,7 +2571,7 @@
         <v>4</v>
       </c>
       <c r="E93" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -2579,7 +2588,7 @@
         <v>4</v>
       </c>
       <c r="E94" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -2596,7 +2605,7 @@
         <v>4</v>
       </c>
       <c r="E95" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -2647,7 +2656,7 @@
         <v>4</v>
       </c>
       <c r="E98" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2664,7 +2673,7 @@
         <v>4</v>
       </c>
       <c r="E99" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2681,7 +2690,7 @@
         <v>4</v>
       </c>
       <c r="E100" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2766,7 +2775,7 @@
         <v>9</v>
       </c>
       <c r="E105" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -2783,7 +2792,7 @@
         <v>9</v>
       </c>
       <c r="E106" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -2868,7 +2877,7 @@
         <v>9</v>
       </c>
       <c r="E111" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -2885,7 +2894,7 @@
         <v>9</v>
       </c>
       <c r="E112" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -2902,7 +2911,7 @@
         <v>9</v>
       </c>
       <c r="E113" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -2953,7 +2962,7 @@
         <v>9</v>
       </c>
       <c r="E116" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -2970,7 +2979,7 @@
         <v>9</v>
       </c>
       <c r="E117" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -2987,7 +2996,7 @@
         <v>9</v>
       </c>
       <c r="E118" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -4738,7 +4747,7 @@
         <v>12</v>
       </c>
       <c r="E221" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
@@ -4755,7 +4764,7 @@
         <v>4</v>
       </c>
       <c r="E222" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -4772,7 +4781,7 @@
         <v>9</v>
       </c>
       <c r="E223" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
committing changes so fix merge
</commit_message>
<xml_diff>
--- a/data/regions.xlsx
+++ b/data/regions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\komickn\Documents\src\CTC_Analysis\chinook_sport_central\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5DE1832-0CBD-455D-8C5F-4DEBE7EEB497}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{574D2E9B-DA83-4AA9-81C2-AEF4476D2926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0E6B1A2C-CD49-44AB-BFC0-F567D14E751E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0E6B1A2C-CD49-44AB-BFC0-F567D14E751E}"/>
   </bookViews>
   <sheets>
     <sheet name="Area" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="770" uniqueCount="196">
   <si>
     <t>AREA</t>
   </si>
@@ -618,6 +618,15 @@
   </si>
   <si>
     <t>NWCVI S SUMMER ISBM</t>
+  </si>
+  <si>
+    <t>NBC ISBM S FALL</t>
+  </si>
+  <si>
+    <t>NBC ISBM S SPRING</t>
+  </si>
+  <si>
+    <t>NBC ISBM S SUMMER</t>
   </si>
 </sst>
 </file>
@@ -972,7 +981,7 @@
   <dimension ref="A1:E256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C256" sqref="C256:D256"/>
+      <selection activeCell="F95" sqref="F95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2154,7 +2163,7 @@
         <v>12</v>
       </c>
       <c r="E69" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -2171,7 +2180,7 @@
         <v>12</v>
       </c>
       <c r="E70" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
@@ -2256,7 +2265,7 @@
         <v>12</v>
       </c>
       <c r="E75" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -2273,7 +2282,7 @@
         <v>12</v>
       </c>
       <c r="E76" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
@@ -2290,7 +2299,7 @@
         <v>12</v>
       </c>
       <c r="E77" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
@@ -2341,7 +2350,7 @@
         <v>12</v>
       </c>
       <c r="E80" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -2358,7 +2367,7 @@
         <v>12</v>
       </c>
       <c r="E81" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -2375,7 +2384,7 @@
         <v>12</v>
       </c>
       <c r="E82" t="s">
-        <v>185</v>
+        <v>193</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -2460,7 +2469,7 @@
         <v>4</v>
       </c>
       <c r="E87" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -2477,7 +2486,7 @@
         <v>4</v>
       </c>
       <c r="E88" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
@@ -2562,7 +2571,7 @@
         <v>4</v>
       </c>
       <c r="E93" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -2579,7 +2588,7 @@
         <v>4</v>
       </c>
       <c r="E94" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -2596,7 +2605,7 @@
         <v>4</v>
       </c>
       <c r="E95" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -2647,7 +2656,7 @@
         <v>4</v>
       </c>
       <c r="E98" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2664,7 +2673,7 @@
         <v>4</v>
       </c>
       <c r="E99" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -2681,7 +2690,7 @@
         <v>4</v>
       </c>
       <c r="E100" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -2766,7 +2775,7 @@
         <v>9</v>
       </c>
       <c r="E105" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
@@ -2783,7 +2792,7 @@
         <v>9</v>
       </c>
       <c r="E106" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
@@ -2868,7 +2877,7 @@
         <v>9</v>
       </c>
       <c r="E111" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.25">
@@ -2885,7 +2894,7 @@
         <v>9</v>
       </c>
       <c r="E112" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
@@ -2902,7 +2911,7 @@
         <v>9</v>
       </c>
       <c r="E113" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -2953,7 +2962,7 @@
         <v>9</v>
       </c>
       <c r="E116" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -2970,7 +2979,7 @@
         <v>9</v>
       </c>
       <c r="E117" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -2987,7 +2996,7 @@
         <v>9</v>
       </c>
       <c r="E118" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -4738,7 +4747,7 @@
         <v>12</v>
       </c>
       <c r="E221" t="s">
-        <v>173</v>
+        <v>193</v>
       </c>
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.25">
@@ -4755,7 +4764,7 @@
         <v>4</v>
       </c>
       <c r="E222" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.25">
@@ -4772,7 +4781,7 @@
         <v>9</v>
       </c>
       <c r="E223" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>